<commit_message>
Updated code to allow for multiple types of RE
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB469BA-4C05-5D49-B33A-86BB2F70064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5039EA91-5BAC-B840-B3F9-A2992846F7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="25720" windowHeight="14700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="25720" windowHeight="14700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
     <sheet name="fuel_tank_costs" sheetId="6" r:id="rId2"/>
     <sheet name="pv_costs" sheetId="3" r:id="rId3"/>
-    <sheet name="battery_costs" sheetId="4" r:id="rId4"/>
-    <sheet name="om_costs" sheetId="11" r:id="rId5"/>
+    <sheet name="mre_costs" sheetId="13" r:id="rId4"/>
+    <sheet name="battery_costs" sheetId="4" r:id="rId5"/>
+    <sheet name="om_costs" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>$/W</t>
   </si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t>Full Load (gal/hr)</t>
+  </si>
+  <si>
+    <t>Tidal</t>
+  </si>
+  <si>
+    <t>$/turbine-yr</t>
   </si>
 </sst>
 </file>
@@ -158,10 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,13 +178,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1023,7 +1022,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+      <c r="A2" s="6">
         <v>250</v>
       </c>
       <c r="B2">
@@ -1031,7 +1030,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="6">
         <v>500</v>
       </c>
       <c r="B3">
@@ -1039,7 +1038,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="6">
         <v>1000</v>
       </c>
       <c r="B4">
@@ -1047,7 +1046,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="6">
         <v>2000</v>
       </c>
       <c r="B5">
@@ -1055,7 +1054,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="6">
         <v>3000</v>
       </c>
       <c r="B6">
@@ -1063,7 +1062,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+      <c r="A7" s="6">
         <v>4000</v>
       </c>
       <c r="B7">
@@ -1071,7 +1070,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="6">
         <v>5200</v>
       </c>
       <c r="B8">
@@ -1079,7 +1078,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="6">
         <v>6000</v>
       </c>
       <c r="B9">
@@ -1087,7 +1086,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="6">
         <v>8000</v>
       </c>
       <c r="B10">
@@ -1095,7 +1094,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="6">
         <v>10000</v>
       </c>
       <c r="B11">
@@ -1103,7 +1102,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="6">
         <v>12000</v>
       </c>
       <c r="B12">
@@ -1119,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1134,22 +1133,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>100</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="3">
         <v>5000</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>100000</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -1164,7 +1163,7 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -1179,7 +1178,7 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -1194,7 +1193,7 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -1215,6 +1214,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F3B84B-2BCA-7544-901C-DA0ED26D60DE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1232,10 +1256,10 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1243,10 +1267,10 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1254,10 +1278,10 @@
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.52100000000000002</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="2">
         <v>0.40100000000000002</v>
       </c>
     </row>
@@ -1266,12 +1290,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1283,82 +1307,92 @@
     <col min="6" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="2">
         <v>102.65</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <v>0.66900000000000004</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="2">
         <v>2.41</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="2">
         <v>15</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="2">
         <v>18</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="2">
         <v>17.5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="2">
         <v>12.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made updates to main.py, generate_tidal_profile.py, MCOR Prices.xlsx, microgrid_optimizer.py, microgrid_system.py to incorporate MRE costs (not complete)
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monc573\PycharmProjects\MCOR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5039EA91-5BAC-B840-B3F9-A2992846F7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32CB37D-6C4D-4B96-A10D-A1E7914634BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="25720" windowHeight="14700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-186" yWindow="8220" windowWidth="8640" windowHeight="4560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>$/W</t>
   </si>
@@ -130,6 +130,51 @@
   </si>
   <si>
     <t>$/turbine-yr</t>
+  </si>
+  <si>
+    <t>Rated Power (kW)</t>
+  </si>
+  <si>
+    <t>Rotor Diameter (m)</t>
+  </si>
+  <si>
+    <t>Rotors per Turbine</t>
+  </si>
+  <si>
+    <t>Nova Innovation's M100-D</t>
+  </si>
+  <si>
+    <t>Tidal Energy Ltd's Deltastream</t>
+  </si>
+  <si>
+    <t>Alstom's DeepGen</t>
+  </si>
+  <si>
+    <t>Orbital Marine Power's SR200</t>
+  </si>
+  <si>
+    <t>Orbital Marine Power's O2</t>
+  </si>
+  <si>
+    <t>Andritz Hydro's HS1500</t>
+  </si>
+  <si>
+    <t>SIMEC's AR1500</t>
+  </si>
+  <si>
+    <t>RM1</t>
+  </si>
+  <si>
+    <t>RM4</t>
+  </si>
+  <si>
+    <t>RM2</t>
+  </si>
+  <si>
+    <t>Turbine Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device Name </t>
   </si>
 </sst>
 </file>
@@ -165,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -181,6 +226,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,14 +513,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -494,7 +540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>20</v>
       </c>
@@ -514,7 +560,7 @@
         <v>7640</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>30</v>
       </c>
@@ -534,7 +580,7 @@
         <v>11460</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>40</v>
       </c>
@@ -554,7 +600,7 @@
         <v>15280</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>60</v>
       </c>
@@ -574,7 +620,7 @@
         <v>22920</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>75</v>
       </c>
@@ -594,7 +640,7 @@
         <v>28650</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>100</v>
       </c>
@@ -614,7 +660,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>125</v>
       </c>
@@ -634,7 +680,7 @@
         <v>47750</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>135</v>
       </c>
@@ -654,7 +700,7 @@
         <v>51570</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>150</v>
       </c>
@@ -674,7 +720,7 @@
         <v>57300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>175</v>
       </c>
@@ -694,7 +740,7 @@
         <v>66850</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>200</v>
       </c>
@@ -714,7 +760,7 @@
         <v>76400</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>230</v>
       </c>
@@ -734,7 +780,7 @@
         <v>87860</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>250</v>
       </c>
@@ -754,7 +800,7 @@
         <v>95500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>300</v>
       </c>
@@ -774,7 +820,7 @@
         <v>114600</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>350</v>
       </c>
@@ -794,7 +840,7 @@
         <v>133700</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>400</v>
       </c>
@@ -814,7 +860,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>500</v>
       </c>
@@ -834,7 +880,7 @@
         <v>191000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>600</v>
       </c>
@@ -854,7 +900,7 @@
         <v>229200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>750</v>
       </c>
@@ -874,7 +920,7 @@
         <v>286500</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -894,7 +940,7 @@
         <v>382000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>1250</v>
       </c>
@@ -914,7 +960,7 @@
         <v>477500</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>1500</v>
       </c>
@@ -934,7 +980,7 @@
         <v>573000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>1750</v>
       </c>
@@ -954,7 +1000,7 @@
         <v>668500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -974,7 +1020,7 @@
         <v>764000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>2250</v>
       </c>
@@ -1008,12 +1054,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6">
         <v>250</v>
       </c>
@@ -1029,7 +1075,7 @@
         <v>7250.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6">
         <v>500</v>
       </c>
@@ -1037,7 +1083,7 @@
         <v>8815.2199999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6">
         <v>1000</v>
       </c>
@@ -1045,7 +1091,7 @@
         <v>10875.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6">
         <v>2000</v>
       </c>
@@ -1053,7 +1099,7 @@
         <v>16117.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6">
         <v>3000</v>
       </c>
@@ -1061,7 +1107,7 @@
         <v>22849.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6">
         <v>4000</v>
       </c>
@@ -1069,7 +1115,7 @@
         <v>26732.799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6">
         <v>5200</v>
       </c>
@@ -1077,7 +1123,7 @@
         <v>34847.15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6">
         <v>6000</v>
       </c>
@@ -1085,7 +1131,7 @@
         <v>33170.78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6">
         <v>8000</v>
       </c>
@@ -1093,7 +1139,7 @@
         <v>39497.300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6">
         <v>10000</v>
       </c>
@@ -1101,7 +1147,7 @@
         <v>45947.77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6">
         <v>12000</v>
       </c>
@@ -1122,17 +1168,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="19.3125" customWidth="1"/>
+    <col min="2" max="2" width="14.47265625" customWidth="1"/>
+    <col min="3" max="3" width="11.47265625" customWidth="1"/>
+    <col min="4" max="4" width="14.47265625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1193,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1162,7 +1208,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +1223,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1238,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1215,26 +1261,244 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F3B84B-2BCA-7544-901C-DA0ED26D60DE}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="24.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.62890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10000</v>
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>530000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1670000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>4680000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3120000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>4400000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <v>1500</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5670000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>1500</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5670000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>1115</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>35561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>89.51</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>6.45</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>4000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>102500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1246,13 +1510,13 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1294,23 +1558,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.47265625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.68359375" customWidth="1"/>
+    <col min="6" max="6" width="19.47265625" customWidth="1"/>
+    <col min="7" max="7" width="14.3125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1339,7 +1603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1366,7 +1630,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
made updates to main.py, generate_tidal_profile.py, MCOR Prices.xlsx, microgrid_optimizer.py, microgrid_system.py to incorporate MRE costs (complete)
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monc573\PycharmProjects\MCOR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32CB37D-6C4D-4B96-A10D-A1E7914634BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E44D85-E63D-4302-AB13-59E61E6B9A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-186" yWindow="8220" windowWidth="8640" windowHeight="4560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8970" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -141,27 +141,6 @@
     <t>Rotors per Turbine</t>
   </si>
   <si>
-    <t>Nova Innovation's M100-D</t>
-  </si>
-  <si>
-    <t>Tidal Energy Ltd's Deltastream</t>
-  </si>
-  <si>
-    <t>Alstom's DeepGen</t>
-  </si>
-  <si>
-    <t>Orbital Marine Power's SR200</t>
-  </si>
-  <si>
-    <t>Orbital Marine Power's O2</t>
-  </si>
-  <si>
-    <t>Andritz Hydro's HS1500</t>
-  </si>
-  <si>
-    <t>SIMEC's AR1500</t>
-  </si>
-  <si>
     <t>RM1</t>
   </si>
   <si>
@@ -175,6 +154,27 @@
   </si>
   <si>
     <t xml:space="preserve">Device Name </t>
+  </si>
+  <si>
+    <t>Nova Innovation M100-D</t>
+  </si>
+  <si>
+    <t>Tidal Energy Ltd Deltastream</t>
+  </si>
+  <si>
+    <t>Alstom DeepGen</t>
+  </si>
+  <si>
+    <t>Orbital Marine Power SR200</t>
+  </si>
+  <si>
+    <t>Orbital Marine Power O2</t>
+  </si>
+  <si>
+    <t>Andritz Hydro HS1500</t>
+  </si>
+  <si>
+    <t>SIMEC AR1500</t>
   </si>
 </sst>
 </file>
@@ -1264,12 +1264,12 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.62890625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.15625" bestFit="1" customWidth="1"/>
@@ -1278,13 +1278,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>400</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>1500</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>1500</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>1115</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>89.51</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>4000</v>

</xml_diff>

<commit_message>
Updated RM1 specs in costs sheet and added tidal param validation
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monc573\PycharmProjects\MCOR\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E44D85-E63D-4302-AB13-59E61E6B9A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10193E50-967C-E74E-A19C-8F15F1CED247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8970" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="1260" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -226,7 +226,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,14 +512,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -540,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -560,7 +559,7 @@
         <v>7640</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>30</v>
       </c>
@@ -580,7 +579,7 @@
         <v>11460</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>40</v>
       </c>
@@ -600,7 +599,7 @@
         <v>15280</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>60</v>
       </c>
@@ -620,7 +619,7 @@
         <v>22920</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
@@ -640,7 +639,7 @@
         <v>28650</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -660,7 +659,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
@@ -680,7 +679,7 @@
         <v>47750</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>135</v>
       </c>
@@ -700,7 +699,7 @@
         <v>51570</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>150</v>
       </c>
@@ -720,7 +719,7 @@
         <v>57300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>175</v>
       </c>
@@ -740,7 +739,7 @@
         <v>66850</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
@@ -760,7 +759,7 @@
         <v>76400</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>230</v>
       </c>
@@ -780,7 +779,7 @@
         <v>87860</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>250</v>
       </c>
@@ -800,7 +799,7 @@
         <v>95500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>300</v>
       </c>
@@ -820,7 +819,7 @@
         <v>114600</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>350</v>
       </c>
@@ -840,7 +839,7 @@
         <v>133700</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>400</v>
       </c>
@@ -860,7 +859,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>500</v>
       </c>
@@ -880,7 +879,7 @@
         <v>191000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>600</v>
       </c>
@@ -900,7 +899,7 @@
         <v>229200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>750</v>
       </c>
@@ -920,7 +919,7 @@
         <v>286500</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -940,7 +939,7 @@
         <v>382000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1250</v>
       </c>
@@ -960,7 +959,7 @@
         <v>477500</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1500</v>
       </c>
@@ -980,7 +979,7 @@
         <v>573000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1750</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>668500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>764000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2250</v>
       </c>
@@ -1054,12 +1053,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83984375" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>250</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>7250.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>500</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>8815.2199999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1000</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>10875.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2000</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>16117.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>3000</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>22849.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>4000</v>
       </c>
@@ -1115,7 +1114,7 @@
         <v>26732.799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>5200</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>34847.15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>6000</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>33170.78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8000</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>39497.300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10000</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>45947.77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>12000</v>
       </c>
@@ -1168,17 +1167,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.3125" customWidth="1"/>
-    <col min="2" max="2" width="14.47265625" customWidth="1"/>
-    <col min="3" max="3" width="11.47265625" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1192,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1207,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1223,7 +1222,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1238,7 +1237,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1264,19 +1263,19 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.62890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1296,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1312,11 +1311,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2">
         <v>530000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1332,11 +1331,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3">
         <v>1670000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1352,11 +1351,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4">
         <v>4680000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1372,11 +1371,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5">
         <v>3120000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1392,11 +1391,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6">
         <v>4400000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1412,11 +1411,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7">
         <v>5670000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1432,11 +1431,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8">
         <v>5670000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1447,16 +1446,16 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9">
         <v>35561</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1472,11 +1471,11 @@
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10">
         <v>3189</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1492,7 +1491,7 @@
       <c r="E11">
         <v>4</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11">
         <v>102500</v>
       </c>
     </row>
@@ -1510,13 +1509,13 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1562,19 +1561,19 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.47265625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.68359375" customWidth="1"/>
-    <col min="6" max="6" width="19.47265625" customWidth="1"/>
-    <col min="7" max="7" width="14.3125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
updated RM turbine prices, and RM2 to 90kW
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monc573\PycharmProjects\MCOR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10193E50-967C-E74E-A19C-8F15F1CED247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBCB6BC-9BE4-4BD7-9FCE-01E1BD9019D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="1260" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -512,14 +512,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -539,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>20</v>
       </c>
@@ -559,7 +559,7 @@
         <v>7640</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>30</v>
       </c>
@@ -579,7 +579,7 @@
         <v>11460</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>40</v>
       </c>
@@ -599,7 +599,7 @@
         <v>15280</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>60</v>
       </c>
@@ -619,7 +619,7 @@
         <v>22920</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>75</v>
       </c>
@@ -639,7 +639,7 @@
         <v>28650</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>100</v>
       </c>
@@ -659,7 +659,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>125</v>
       </c>
@@ -679,7 +679,7 @@
         <v>47750</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>135</v>
       </c>
@@ -699,7 +699,7 @@
         <v>51570</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>150</v>
       </c>
@@ -719,7 +719,7 @@
         <v>57300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>175</v>
       </c>
@@ -739,7 +739,7 @@
         <v>66850</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>200</v>
       </c>
@@ -759,7 +759,7 @@
         <v>76400</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>230</v>
       </c>
@@ -779,7 +779,7 @@
         <v>87860</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>250</v>
       </c>
@@ -799,7 +799,7 @@
         <v>95500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>300</v>
       </c>
@@ -819,7 +819,7 @@
         <v>114600</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>350</v>
       </c>
@@ -839,7 +839,7 @@
         <v>133700</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>400</v>
       </c>
@@ -859,7 +859,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>500</v>
       </c>
@@ -879,7 +879,7 @@
         <v>191000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>600</v>
       </c>
@@ -899,7 +899,7 @@
         <v>229200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>750</v>
       </c>
@@ -919,7 +919,7 @@
         <v>286500</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -939,7 +939,7 @@
         <v>382000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>1250</v>
       </c>
@@ -959,7 +959,7 @@
         <v>477500</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>1500</v>
       </c>
@@ -979,7 +979,7 @@
         <v>573000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>1750</v>
       </c>
@@ -999,7 +999,7 @@
         <v>668500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>764000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>2250</v>
       </c>
@@ -1053,12 +1053,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6">
         <v>250</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>7250.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6">
         <v>500</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>8815.2199999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6">
         <v>1000</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>10875.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6">
         <v>2000</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>16117.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6">
         <v>3000</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>22849.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6">
         <v>4000</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>26732.799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6">
         <v>5200</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>34847.15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6">
         <v>6000</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>33170.78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6">
         <v>8000</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>39497.300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6">
         <v>10000</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>45947.77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6">
         <v>12000</v>
       </c>
@@ -1167,17 +1167,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="19.3125" customWidth="1"/>
+    <col min="2" max="2" width="14.47265625" customWidth="1"/>
+    <col min="3" max="3" width="11.47265625" customWidth="1"/>
+    <col min="4" max="4" width="14.47265625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1263,19 +1263,19 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.68359375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>530000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>1670000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>4680000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>3120000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>5670000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>5670000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1452,15 +1452,15 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>35561</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4360000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10">
-        <v>89.51</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1472,10 +1472,10 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>3189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>102500</v>
+        <v>15000000</v>
       </c>
     </row>
   </sheetData>
@@ -1509,13 +1509,13 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1561,19 +1561,19 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.47265625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.68359375" customWidth="1"/>
+    <col min="6" max="6" width="19.47265625" customWidth="1"/>
+    <col min="7" max="7" width="14.3125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
updated MRE O&M with costs from the literature
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monc573\PycharmProjects\MCOR\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBCB6BC-9BE4-4BD7-9FCE-01E1BD9019D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B367971F-265C-884F-AE61-CFAB67A136D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28480" yWindow="14220" windowWidth="23240" windowHeight="14000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>$/W</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Tidal</t>
-  </si>
-  <si>
-    <t>$/turbine-yr</t>
   </si>
   <si>
     <t>Rated Power (kW)</t>
@@ -512,14 +509,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -539,7 +536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -559,7 +556,7 @@
         <v>7640</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>30</v>
       </c>
@@ -579,7 +576,7 @@
         <v>11460</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>40</v>
       </c>
@@ -599,7 +596,7 @@
         <v>15280</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>60</v>
       </c>
@@ -619,7 +616,7 @@
         <v>22920</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
@@ -639,7 +636,7 @@
         <v>28650</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -659,7 +656,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
@@ -679,7 +676,7 @@
         <v>47750</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>135</v>
       </c>
@@ -699,7 +696,7 @@
         <v>51570</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>150</v>
       </c>
@@ -719,7 +716,7 @@
         <v>57300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>175</v>
       </c>
@@ -739,7 +736,7 @@
         <v>66850</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
@@ -759,7 +756,7 @@
         <v>76400</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>230</v>
       </c>
@@ -779,7 +776,7 @@
         <v>87860</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>250</v>
       </c>
@@ -799,7 +796,7 @@
         <v>95500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>300</v>
       </c>
@@ -819,7 +816,7 @@
         <v>114600</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>350</v>
       </c>
@@ -839,7 +836,7 @@
         <v>133700</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>400</v>
       </c>
@@ -859,7 +856,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>500</v>
       </c>
@@ -879,7 +876,7 @@
         <v>191000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>600</v>
       </c>
@@ -899,7 +896,7 @@
         <v>229200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>750</v>
       </c>
@@ -919,7 +916,7 @@
         <v>286500</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -939,7 +936,7 @@
         <v>382000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1250</v>
       </c>
@@ -959,7 +956,7 @@
         <v>477500</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1500</v>
       </c>
@@ -979,7 +976,7 @@
         <v>573000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1750</v>
       </c>
@@ -999,7 +996,7 @@
         <v>668500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -1019,7 +1016,7 @@
         <v>764000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2250</v>
       </c>
@@ -1053,12 +1050,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83984375" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>250</v>
       </c>
@@ -1074,7 +1071,7 @@
         <v>7250.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>500</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>8815.2199999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1000</v>
       </c>
@@ -1090,7 +1087,7 @@
         <v>10875.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2000</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>16117.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>3000</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>22849.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>4000</v>
       </c>
@@ -1114,7 +1111,7 @@
         <v>26732.799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>5200</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>34847.15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>6000</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>33170.78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8000</v>
       </c>
@@ -1138,7 +1135,7 @@
         <v>39497.300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10000</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>45947.77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>12000</v>
       </c>
@@ -1167,17 +1164,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.3125" customWidth="1"/>
-    <col min="2" max="2" width="14.47265625" customWidth="1"/>
-    <col min="3" max="3" width="11.47265625" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1189,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1207,7 +1204,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1219,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1234,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1263,41 +1260,41 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1315,9 +1312,9 @@
         <v>530000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>400</v>
@@ -1335,9 +1332,9 @@
         <v>1670000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -1355,9 +1352,9 @@
         <v>4680000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -1375,9 +1372,9 @@
         <v>3120000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -1395,9 +1392,9 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>1500</v>
@@ -1415,9 +1412,9 @@
         <v>5670000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>1500</v>
@@ -1435,9 +1432,9 @@
         <v>5670000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>1115</v>
@@ -1455,9 +1452,9 @@
         <v>4360000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>90</v>
@@ -1475,9 +1472,9 @@
         <v>580000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>4000</v>
@@ -1509,13 +1506,13 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1558,22 +1555,22 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.47265625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.68359375" customWidth="1"/>
-    <col min="6" max="6" width="19.47265625" customWidth="1"/>
-    <col min="7" max="7" width="14.3125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1626,10 +1623,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1655,7 +1652,7 @@
         <v>12.5</v>
       </c>
       <c r="I3" s="2">
-        <v>100</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small updates to pv sizing alg, added units to pv costs sheet
</commit_message>
<xml_diff>
--- a/data/MCOR Prices.xlsx
+++ b/data/MCOR Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newm562/repos/areit/mcor_public/MCOR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B367971F-265C-884F-AE61-CFAB67A136D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC71F300-8911-8F44-A10C-4AB0AF932452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28480" yWindow="14220" windowWidth="23240" windowHeight="14000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>$/W</t>
   </si>
@@ -1158,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1189,65 +1189,80 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2.78</v>
-      </c>
-      <c r="C2">
-        <v>1.64</v>
-      </c>
-      <c r="D2">
-        <v>0.83</v>
-      </c>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>2.97</v>
+        <v>2.78</v>
       </c>
       <c r="C3">
-        <v>1.75</v>
+        <v>1.64</v>
       </c>
       <c r="D3">
-        <v>0.89</v>
+        <v>0.83</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>2.65</v>
+        <v>2.97</v>
       </c>
       <c r="C4">
-        <v>1.56</v>
+        <v>1.75</v>
       </c>
       <c r="D4">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>3.15</v>
+        <v>2.65</v>
       </c>
       <c r="C5">
-        <v>1.86</v>
+        <v>1.56</v>
       </c>
       <c r="D5">
         <v>0.83</v>
       </c>
       <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>3.15</v>
+      </c>
+      <c r="C6">
+        <v>1.86</v>
+      </c>
+      <c r="D6">
+        <v>0.83</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1259,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F3B84B-2BCA-7544-901C-DA0ED26D60DE}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>